<commit_message>
Encore des soucis de titres
</commit_message>
<xml_diff>
--- a/Unverified multiformat sources/Importations Levant 1771.xlsx
+++ b/Unverified multiformat sources/Importations Levant 1771.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10523"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumedaudin/Documents/Recherche/Commerce International Français XVIIIe.xls/Balance du commerce/Retranscriptions_Commerce_France/toflit18_data_GIT/Unverified multiformat sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D647038-7289-F443-9230-232FC31E5923}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB202CC-7448-834C-958A-F6DB4EDFF057}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$B$1:$X$23</definedName>
   </definedNames>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179017" iterateDelta="1E-4"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -649,9 +649,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>problem</t>
-  </si>
-  <si>
     <t>remarks</t>
   </si>
   <si>
@@ -662,6 +659,9 @@
   </si>
   <si>
     <t>Importations</t>
+  </si>
+  <si>
+    <t>probleme</t>
   </si>
 </sst>
 </file>
@@ -3660,7 +3660,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="1368" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3693,18 +3693,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -4069,8 +4057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1510"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4166,10 +4154,10 @@
         <v>169</v>
       </c>
       <c r="W1" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="X1" s="30" t="s">
         <v>170</v>
-      </c>
-      <c r="X1" s="30" t="s">
-        <v>171</v>
       </c>
       <c r="Y1" s="29" t="s">
         <v>154</v>
@@ -4186,16 +4174,16 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F2" s="4">
         <v>1771</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="2">
@@ -4257,16 +4245,16 @@
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F3" s="4">
         <v>1771</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="2">
@@ -4328,16 +4316,16 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F4" s="4">
         <v>1771</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="2">
@@ -4399,16 +4387,16 @@
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F5" s="4">
         <v>1771</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="2">
@@ -4470,16 +4458,16 @@
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F6" s="4">
         <v>1771</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="2">
@@ -4539,16 +4527,16 @@
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F7" s="4">
         <v>1771</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="2">
@@ -4608,16 +4596,16 @@
         <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F8" s="4">
         <v>1771</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="2">
@@ -4679,16 +4667,16 @@
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F9" s="4">
         <v>1771</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="2">
@@ -4748,16 +4736,16 @@
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F10" s="4">
         <v>1771</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="2">
@@ -4819,16 +4807,16 @@
         <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F11" s="4">
         <v>1771</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="2">
@@ -4890,16 +4878,16 @@
         <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F12" s="4">
         <v>1771</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="2">
@@ -4959,16 +4947,16 @@
         <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F13" s="4">
         <v>1771</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="2">
@@ -5030,16 +5018,16 @@
         <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F14" s="4">
         <v>1771</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="2">
@@ -5099,16 +5087,16 @@
         <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F15" s="4">
         <v>1771</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="2">
@@ -5168,16 +5156,16 @@
         <v>8</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F16" s="4">
         <v>1771</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="2">
@@ -5239,16 +5227,16 @@
         <v>8</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F17" s="4">
         <v>1771</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="2">
@@ -5310,16 +5298,16 @@
         <v>8</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F18" s="4">
         <v>1771</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="2">
@@ -5379,16 +5367,16 @@
         <v>8</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F19" s="4">
         <v>1771</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="2">
@@ -5450,16 +5438,16 @@
         <v>8</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F20" s="4">
         <v>1771</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="2">
@@ -5521,16 +5509,16 @@
         <v>8</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F21" s="4">
         <v>1771</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="2">
@@ -5590,16 +5578,16 @@
         <v>8</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F22" s="4">
         <v>1771</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="2">
@@ -5659,16 +5647,16 @@
         <v>8</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F23" s="4">
         <v>1771</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="2">
@@ -5730,16 +5718,16 @@
         <v>8</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F24" s="4">
         <v>1771</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="2">
@@ -5801,16 +5789,16 @@
         <v>8</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F25" s="4">
         <v>1771</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="2">
@@ -5870,16 +5858,16 @@
         <v>8</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F26" s="4">
         <v>1771</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="2">
@@ -5939,16 +5927,16 @@
         <v>8</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F27" s="4">
         <v>1771</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="2">
@@ -6008,16 +5996,16 @@
         <v>8</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F28" s="4">
         <v>1771</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="2">
@@ -6077,16 +6065,16 @@
         <v>8</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F29" s="4">
         <v>1771</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="2">
@@ -6148,16 +6136,16 @@
         <v>8</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F30" s="4">
         <v>1771</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="2">
@@ -6217,16 +6205,16 @@
         <v>8</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F31" s="4">
         <v>1771</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="2">
@@ -6286,16 +6274,16 @@
         <v>8</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F32" s="4">
         <v>1771</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="2">
@@ -6355,16 +6343,16 @@
         <v>8</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F33" s="4">
         <v>1771</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="2">
@@ -6426,16 +6414,16 @@
         <v>8</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F34" s="4">
         <v>1771</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="2">
@@ -6495,16 +6483,16 @@
         <v>8</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F35" s="4">
         <v>1771</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="2">
@@ -6566,16 +6554,16 @@
         <v>8</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F36" s="4">
         <v>1771</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H36" s="7"/>
       <c r="I36" s="2">
@@ -6635,16 +6623,16 @@
         <v>8</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F37" s="4">
         <v>1771</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H37" s="7"/>
       <c r="I37" s="2">
@@ -6706,16 +6694,16 @@
         <v>8</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F38" s="4">
         <v>1771</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="2">
@@ -6775,16 +6763,16 @@
         <v>8</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F39" s="4">
         <v>1771</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H39" s="7"/>
       <c r="I39" s="2">
@@ -6846,16 +6834,16 @@
         <v>8</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F40" s="4">
         <v>1771</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H40" s="7"/>
       <c r="I40" s="2">
@@ -6915,16 +6903,16 @@
         <v>8</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F41" s="4">
         <v>1771</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H41" s="7"/>
       <c r="I41" s="2">
@@ -6984,16 +6972,16 @@
         <v>8</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F42" s="4">
         <v>1771</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H42" s="7"/>
       <c r="I42" s="2">
@@ -7055,16 +7043,16 @@
         <v>8</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F43" s="4">
         <v>1771</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H43" s="7"/>
       <c r="I43" s="2">
@@ -7126,16 +7114,16 @@
         <v>8</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F44" s="4">
         <v>1771</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="2">
@@ -7195,16 +7183,16 @@
         <v>8</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F45" s="4">
         <v>1771</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="2">
@@ -7264,16 +7252,16 @@
         <v>8</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F46" s="4">
         <v>1771</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H46" s="7"/>
       <c r="I46" s="2">
@@ -7335,16 +7323,16 @@
         <v>8</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F47" s="4">
         <v>1771</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H47" s="7"/>
       <c r="I47" s="2">
@@ -7404,16 +7392,16 @@
         <v>8</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F48" s="4">
         <v>1771</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="2">
@@ -7475,16 +7463,16 @@
         <v>8</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F49" s="4">
         <v>1771</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H49" s="7"/>
       <c r="I49" s="2">
@@ -7540,16 +7528,16 @@
         <v>8</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F50" s="4">
         <v>1771</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="2">
@@ -7609,16 +7597,16 @@
         <v>8</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F51" s="4">
         <v>1771</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="2">
@@ -7678,16 +7666,16 @@
         <v>8</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F52" s="4">
         <v>1771</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" s="2">
@@ -7747,16 +7735,16 @@
         <v>8</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F53" s="4">
         <v>1771</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H53" s="7"/>
       <c r="I53" s="2">
@@ -7816,16 +7804,16 @@
         <v>8</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F54" s="4">
         <v>1771</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="2">
@@ -7887,16 +7875,16 @@
         <v>8</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F55" s="4">
         <v>1771</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H55" s="7"/>
       <c r="I55" s="2">
@@ -7956,16 +7944,16 @@
         <v>8</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F56" s="4">
         <v>1771</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="2">
@@ -8027,16 +8015,16 @@
         <v>8</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F57" s="4">
         <v>1771</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H57" s="7"/>
       <c r="I57" s="2">
@@ -8098,16 +8086,16 @@
         <v>8</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F58" s="4">
         <v>1771</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H58" s="7"/>
       <c r="I58" s="2">
@@ -8167,16 +8155,16 @@
         <v>8</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F59" s="4">
         <v>1771</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H59" s="7"/>
       <c r="I59" s="2">
@@ -8238,16 +8226,16 @@
         <v>8</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F60" s="4">
         <v>1771</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="2">
@@ -8307,16 +8295,16 @@
         <v>8</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F61" s="4">
         <v>1771</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H61" s="7"/>
       <c r="I61" s="2">
@@ -8376,16 +8364,16 @@
         <v>8</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F62" s="4">
         <v>1771</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H62" s="7"/>
       <c r="I62" s="2">
@@ -8445,16 +8433,16 @@
         <v>8</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F63" s="4">
         <v>1771</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H63" s="7"/>
       <c r="I63" s="2">
@@ -8514,16 +8502,16 @@
         <v>8</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F64" s="4">
         <v>1771</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H64" s="7"/>
       <c r="I64" s="2">
@@ -8583,16 +8571,16 @@
         <v>8</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F65" s="4">
         <v>1771</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H65" s="7"/>
       <c r="I65" s="2">
@@ -8654,16 +8642,16 @@
         <v>8</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F66" s="4">
         <v>1771</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H66" s="7"/>
       <c r="I66" s="2">
@@ -8723,16 +8711,16 @@
         <v>8</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F67" s="4">
         <v>1771</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H67" s="7"/>
       <c r="I67" s="2">
@@ -8792,16 +8780,16 @@
         <v>8</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F68" s="4">
         <v>1771</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H68" s="7"/>
       <c r="I68" s="2">
@@ -8861,16 +8849,16 @@
         <v>8</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F69" s="4">
         <v>1771</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H69" s="7"/>
       <c r="I69" s="2">
@@ -8930,16 +8918,16 @@
         <v>8</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F70" s="4">
         <v>1771</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H70" s="7"/>
       <c r="I70" s="2">
@@ -8999,16 +8987,16 @@
         <v>8</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F71" s="4">
         <v>1771</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H71" s="7"/>
       <c r="I71" s="2">
@@ -9068,16 +9056,16 @@
         <v>8</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F72" s="4">
         <v>1771</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H72" s="7"/>
       <c r="I72" s="2">
@@ -9137,16 +9125,16 @@
         <v>8</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F73" s="4">
         <v>1771</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H73" s="7"/>
       <c r="I73" s="2">
@@ -9206,16 +9194,16 @@
         <v>8</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F74" s="4">
         <v>1771</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H74" s="7"/>
       <c r="I74" s="2">
@@ -9275,16 +9263,16 @@
         <v>8</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F75" s="4">
         <v>1771</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H75" s="7"/>
       <c r="I75" s="2">
@@ -9344,16 +9332,16 @@
         <v>8</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F76" s="4">
         <v>1771</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H76" s="7"/>
       <c r="I76" s="2">
@@ -9413,16 +9401,16 @@
         <v>8</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F77" s="4">
         <v>1771</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H77" s="7"/>
       <c r="I77" s="2">
@@ -9482,16 +9470,16 @@
         <v>8</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F78" s="4">
         <v>1771</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H78" s="7"/>
       <c r="I78" s="2">
@@ -9551,16 +9539,16 @@
         <v>8</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F79" s="4">
         <v>1771</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H79" s="7"/>
       <c r="I79" s="2">
@@ -9620,16 +9608,16 @@
         <v>8</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F80" s="4">
         <v>1771</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H80" s="7"/>
       <c r="I80" s="2">
@@ -9689,16 +9677,16 @@
         <v>8</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F81" s="4">
         <v>1771</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H81" s="7"/>
       <c r="I81" s="2">
@@ -9758,16 +9746,16 @@
         <v>8</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F82" s="4">
         <v>1771</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H82" s="7"/>
       <c r="I82" s="2">
@@ -9829,16 +9817,16 @@
         <v>8</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F83" s="4">
         <v>1771</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H83" s="7"/>
       <c r="I83" s="2">
@@ -9898,16 +9886,16 @@
         <v>8</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F84" s="4">
         <v>1771</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H84" s="7"/>
       <c r="I84" s="2">
@@ -9967,16 +9955,16 @@
         <v>8</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F85" s="4">
         <v>1771</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H85" s="7"/>
       <c r="I85" s="2">
@@ -10038,16 +10026,16 @@
         <v>8</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F86" s="4">
         <v>1771</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H86" s="7"/>
       <c r="I86" s="2">
@@ -10109,16 +10097,16 @@
         <v>8</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F87" s="4">
         <v>1771</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H87" s="7"/>
       <c r="I87" s="2">
@@ -10178,16 +10166,16 @@
         <v>8</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F88" s="4">
         <v>1771</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H88" s="7"/>
       <c r="I88" s="2">
@@ -10249,16 +10237,16 @@
         <v>8</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F89" s="4">
         <v>1771</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H89" s="7"/>
       <c r="I89" s="2">
@@ -10320,16 +10308,16 @@
         <v>8</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F90" s="4">
         <v>1771</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H90" s="7"/>
       <c r="I90" s="2">
@@ -10389,16 +10377,16 @@
         <v>8</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F91" s="4">
         <v>1771</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H91" s="7"/>
       <c r="I91" s="2">
@@ -10460,16 +10448,16 @@
         <v>8</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F92" s="4">
         <v>1771</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H92" s="7"/>
       <c r="I92" s="2">
@@ -10529,16 +10517,16 @@
         <v>8</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F93" s="4">
         <v>1771</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H93" s="7"/>
       <c r="I93" s="2">
@@ -10598,16 +10586,16 @@
         <v>8</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F94" s="4">
         <v>1771</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H94" s="7"/>
       <c r="I94" s="2">
@@ -10667,16 +10655,16 @@
         <v>8</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F95" s="4">
         <v>1771</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H95" s="7"/>
       <c r="I95" s="2">
@@ -10736,16 +10724,16 @@
         <v>8</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F96" s="4">
         <v>1771</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H96" s="7"/>
       <c r="I96" s="2">
@@ -10807,16 +10795,16 @@
         <v>8</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F97" s="4">
         <v>1771</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H97" s="7"/>
       <c r="I97" s="2">
@@ -10878,16 +10866,16 @@
         <v>8</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F98" s="4">
         <v>1771</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H98" s="7"/>
       <c r="I98" s="2">
@@ -10947,16 +10935,16 @@
         <v>8</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F99" s="4">
         <v>1771</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H99" s="7"/>
       <c r="I99" s="2">
@@ -11016,16 +11004,16 @@
         <v>8</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F100" s="4">
         <v>1771</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H100" s="7"/>
       <c r="I100" s="2">
@@ -11085,16 +11073,16 @@
         <v>8</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F101" s="4">
         <v>1771</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H101" s="7"/>
       <c r="I101" s="2">
@@ -11156,16 +11144,16 @@
         <v>8</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F102" s="4">
         <v>1771</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H102" s="7"/>
       <c r="I102" s="2">
@@ -11227,16 +11215,16 @@
         <v>8</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F103" s="4">
         <v>1771</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H103" s="7"/>
       <c r="I103" s="2">
@@ -11296,16 +11284,16 @@
         <v>8</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F104" s="4">
         <v>1771</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H104" s="7"/>
       <c r="I104" s="2">
@@ -11365,16 +11353,16 @@
         <v>8</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F105" s="4">
         <v>1771</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H105" s="7"/>
       <c r="I105" s="2">
@@ -11434,16 +11422,16 @@
         <v>8</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F106" s="4">
         <v>1771</v>
       </c>
       <c r="G106" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H106" s="7"/>
       <c r="I106" s="2">
@@ -11503,16 +11491,16 @@
         <v>8</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F107" s="4">
         <v>1771</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H107" s="7"/>
       <c r="I107" s="2">
@@ -11574,16 +11562,16 @@
         <v>8</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F108" s="4">
         <v>1771</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H108" s="7"/>
       <c r="I108" s="2">
@@ -11645,16 +11633,16 @@
         <v>8</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F109" s="4">
         <v>1771</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H109" s="7"/>
       <c r="I109" s="2">
@@ -11714,16 +11702,16 @@
         <v>8</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F110" s="4">
         <v>1771</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H110" s="7"/>
       <c r="I110" s="2">
@@ -11783,16 +11771,16 @@
         <v>8</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F111" s="4">
         <v>1771</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H111" s="7"/>
       <c r="I111" s="2">
@@ -11852,16 +11840,16 @@
         <v>8</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F112" s="4">
         <v>1771</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H112" s="7"/>
       <c r="I112" s="2">
@@ -11923,16 +11911,16 @@
         <v>8</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F113" s="4">
         <v>1771</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H113" s="7"/>
       <c r="I113" s="2">
@@ -11994,16 +11982,16 @@
         <v>8</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F114" s="4">
         <v>1771</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H114" s="7"/>
       <c r="I114" s="2">
@@ -12063,16 +12051,16 @@
         <v>8</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F115" s="4">
         <v>1771</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H115" s="7"/>
       <c r="I115" s="2">
@@ -12132,16 +12120,16 @@
         <v>8</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F116" s="4">
         <v>1771</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H116" s="7"/>
       <c r="I116" s="2"/>
@@ -12199,16 +12187,16 @@
         <v>8</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F117" s="4">
         <v>1771</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H117" s="7"/>
       <c r="I117" s="2"/>
@@ -12266,16 +12254,16 @@
         <v>8</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F118" s="4">
         <v>1771</v>
       </c>
       <c r="G118" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H118" s="7"/>
       <c r="I118" s="2"/>
@@ -12333,16 +12321,16 @@
         <v>8</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F119" s="4">
         <v>1771</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H119" s="7"/>
       <c r="I119" s="2"/>
@@ -12400,16 +12388,16 @@
         <v>8</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F120" s="4">
         <v>1771</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H120" s="7"/>
       <c r="I120" s="2"/>
@@ -12469,16 +12457,16 @@
         <v>8</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F121" s="4">
         <v>1771</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H121" s="7"/>
       <c r="I121" s="2"/>
@@ -12536,16 +12524,16 @@
         <v>8</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F122" s="4">
         <v>1771</v>
       </c>
       <c r="G122" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H122" s="7"/>
       <c r="I122" s="2"/>
@@ -12603,16 +12591,16 @@
         <v>8</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F123" s="4">
         <v>1771</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H123" s="7"/>
       <c r="I123" s="2"/>
@@ -12672,16 +12660,16 @@
         <v>8</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F124" s="4">
         <v>1771</v>
       </c>
       <c r="G124" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H124" s="7"/>
       <c r="I124" s="2"/>
@@ -12741,16 +12729,16 @@
         <v>8</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F125" s="4">
         <v>1771</v>
       </c>
       <c r="G125" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H125" s="7"/>
       <c r="I125" s="2"/>
@@ -12808,16 +12796,16 @@
         <v>8</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F126" s="4">
         <v>1771</v>
       </c>
       <c r="G126" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H126" s="7"/>
       <c r="I126" s="2"/>
@@ -12877,16 +12865,16 @@
         <v>8</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F127" s="4">
         <v>1771</v>
       </c>
       <c r="G127" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H127" s="7"/>
       <c r="I127" s="2"/>
@@ -12946,16 +12934,16 @@
         <v>8</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F128" s="4">
         <v>1771</v>
       </c>
       <c r="G128" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H128" s="7"/>
       <c r="I128" s="2"/>
@@ -13013,16 +13001,16 @@
         <v>8</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F129" s="4">
         <v>1771</v>
       </c>
       <c r="G129" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H129" s="7"/>
       <c r="I129" s="2"/>
@@ -13082,16 +13070,16 @@
         <v>8</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F130" s="4">
         <v>1771</v>
       </c>
       <c r="G130" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H130" s="7"/>
       <c r="I130" s="2"/>
@@ -13151,16 +13139,16 @@
         <v>8</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F131" s="4">
         <v>1771</v>
       </c>
       <c r="G131" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H131" s="7"/>
       <c r="I131" s="2"/>
@@ -13220,16 +13208,16 @@
         <v>8</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F132" s="4">
         <v>1771</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H132" s="7"/>
       <c r="I132" s="2"/>
@@ -13289,16 +13277,16 @@
         <v>8</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F133" s="4">
         <v>1771</v>
       </c>
       <c r="G133" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H133" s="7"/>
       <c r="I133" s="2"/>
@@ -13358,16 +13346,16 @@
         <v>8</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F134" s="4">
         <v>1771</v>
       </c>
       <c r="G134" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H134" s="7"/>
       <c r="I134" s="2"/>
@@ -13425,16 +13413,16 @@
         <v>8</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F135" s="4">
         <v>1771</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H135" s="7"/>
       <c r="I135" s="2"/>
@@ -13492,16 +13480,16 @@
         <v>8</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F136" s="4">
         <v>1771</v>
       </c>
       <c r="G136" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H136" s="7"/>
       <c r="I136" s="2"/>
@@ -13559,16 +13547,16 @@
         <v>8</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F137" s="4">
         <v>1771</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H137" s="7"/>
       <c r="I137" s="2"/>
@@ -13626,16 +13614,16 @@
         <v>8</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F138" s="4">
         <v>1771</v>
       </c>
       <c r="G138" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H138" s="7"/>
       <c r="I138" s="2"/>
@@ -13693,16 +13681,16 @@
         <v>8</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F139" s="4">
         <v>1771</v>
       </c>
       <c r="G139" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H139" s="7"/>
       <c r="I139" s="2"/>
@@ -13760,16 +13748,16 @@
         <v>8</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F140" s="4">
         <v>1771</v>
       </c>
       <c r="G140" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H140" s="7"/>
       <c r="I140" s="2"/>
@@ -13829,16 +13817,16 @@
         <v>8</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F141" s="4">
         <v>1771</v>
       </c>
       <c r="G141" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H141" s="7"/>
       <c r="I141" s="2"/>
@@ -13896,16 +13884,16 @@
         <v>8</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F142" s="4">
         <v>1771</v>
       </c>
       <c r="G142" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H142" s="7"/>
       <c r="I142" s="2"/>
@@ -13963,16 +13951,16 @@
         <v>8</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F143" s="4">
         <v>1771</v>
       </c>
       <c r="G143" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H143" s="7"/>
       <c r="I143" s="2"/>
@@ -14030,16 +14018,16 @@
         <v>8</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F144" s="4">
         <v>1771</v>
       </c>
       <c r="G144" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H144" s="7"/>
       <c r="I144" s="2"/>
@@ -14097,16 +14085,16 @@
         <v>8</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F145" s="4">
         <v>1771</v>
       </c>
       <c r="G145" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H145" s="7"/>
       <c r="I145" s="2"/>
@@ -14164,16 +14152,16 @@
         <v>8</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F146" s="4">
         <v>1771</v>
       </c>
       <c r="G146" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H146" s="7"/>
       <c r="I146" s="2"/>
@@ -14231,16 +14219,16 @@
         <v>8</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F147" s="4">
         <v>1771</v>
       </c>
       <c r="G147" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H147" s="7"/>
       <c r="I147" s="2"/>
@@ -14298,16 +14286,16 @@
         <v>8</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F148" s="4">
         <v>1771</v>
       </c>
       <c r="G148" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H148" s="7"/>
       <c r="I148" s="2"/>
@@ -14365,16 +14353,16 @@
         <v>8</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F149" s="4">
         <v>1771</v>
       </c>
       <c r="G149" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H149" s="7"/>
       <c r="I149" s="2"/>
@@ -14434,16 +14422,16 @@
         <v>8</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F150" s="4">
         <v>1771</v>
       </c>
       <c r="G150" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H150" s="7"/>
       <c r="I150" s="2"/>
@@ -14503,16 +14491,16 @@
         <v>8</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F151" s="4">
         <v>1771</v>
       </c>
       <c r="G151" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H151" s="7"/>
       <c r="I151" s="2"/>
@@ -14570,16 +14558,16 @@
         <v>8</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F152" s="4">
         <v>1771</v>
       </c>
       <c r="G152" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H152" s="7"/>
       <c r="I152" s="2"/>
@@ -14637,16 +14625,16 @@
         <v>8</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F153" s="4">
         <v>1771</v>
       </c>
       <c r="G153" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H153" s="7"/>
       <c r="I153" s="2"/>
@@ -14706,16 +14694,16 @@
         <v>8</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F154" s="4">
         <v>1771</v>
       </c>
       <c r="G154" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H154" s="7"/>
       <c r="I154" s="2"/>
@@ -14775,16 +14763,16 @@
         <v>8</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F155" s="4">
         <v>1771</v>
       </c>
       <c r="G155" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H155" s="7"/>
       <c r="I155" s="2"/>
@@ -14842,16 +14830,16 @@
         <v>8</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F156" s="4">
         <v>1771</v>
       </c>
       <c r="G156" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H156" s="7"/>
       <c r="I156" s="2"/>
@@ -14909,16 +14897,16 @@
         <v>8</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F157" s="4">
         <v>1771</v>
       </c>
       <c r="G157" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H157" s="7"/>
       <c r="I157" s="2"/>
@@ -14978,16 +14966,16 @@
         <v>8</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F158" s="4">
         <v>1771</v>
       </c>
       <c r="G158" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H158" s="7"/>
       <c r="I158" s="2"/>
@@ -15045,16 +15033,16 @@
         <v>8</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F159" s="4">
         <v>1771</v>
       </c>
       <c r="G159" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H159" s="7"/>
       <c r="I159" s="2"/>
@@ -15112,16 +15100,16 @@
         <v>8</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F160" s="4">
         <v>1771</v>
       </c>
       <c r="G160" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H160" s="7"/>
       <c r="I160" s="2"/>
@@ -15179,16 +15167,16 @@
         <v>8</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F161" s="4">
         <v>1771</v>
       </c>
       <c r="G161" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H161" s="7"/>
       <c r="I161" s="2"/>
@@ -15246,16 +15234,16 @@
         <v>8</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F162" s="4">
         <v>1771</v>
       </c>
       <c r="G162" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H162" s="7"/>
       <c r="I162" s="2"/>
@@ -15313,16 +15301,16 @@
         <v>8</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F163" s="4">
         <v>1771</v>
       </c>
       <c r="G163" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H163" s="7"/>
       <c r="I163" s="2"/>
@@ -15382,16 +15370,16 @@
         <v>8</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F164" s="4">
         <v>1771</v>
       </c>
       <c r="G164" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H164" s="7"/>
       <c r="I164" s="2"/>
@@ -15449,16 +15437,16 @@
         <v>8</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F165" s="4">
         <v>1771</v>
       </c>
       <c r="G165" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H165" s="7"/>
       <c r="I165" s="2"/>
@@ -15516,16 +15504,16 @@
         <v>8</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F166" s="4">
         <v>1771</v>
       </c>
       <c r="G166" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H166" s="7"/>
       <c r="I166" s="2"/>
@@ -15583,16 +15571,16 @@
         <v>8</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F167" s="4">
         <v>1771</v>
       </c>
       <c r="G167" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H167" s="7"/>
       <c r="I167" s="2"/>
@@ -15650,16 +15638,16 @@
         <v>8</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F168" s="4">
         <v>1771</v>
       </c>
       <c r="G168" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H168" s="7"/>
       <c r="I168" s="2"/>
@@ -15719,16 +15707,16 @@
         <v>8</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F169" s="4">
         <v>1771</v>
       </c>
       <c r="G169" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H169" s="7"/>
       <c r="I169" s="2"/>
@@ -15786,16 +15774,16 @@
         <v>8</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F170" s="4">
         <v>1771</v>
       </c>
       <c r="G170" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H170" s="7"/>
       <c r="I170" s="2"/>
@@ -15855,16 +15843,16 @@
         <v>8</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F171" s="4">
         <v>1771</v>
       </c>
       <c r="G171" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H171" s="7"/>
       <c r="I171" s="2"/>
@@ -15924,16 +15912,16 @@
         <v>8</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F172" s="4">
         <v>1771</v>
       </c>
       <c r="G172" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H172" s="7"/>
       <c r="I172" s="2"/>
@@ -15991,16 +15979,16 @@
         <v>8</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F173" s="4">
         <v>1771</v>
       </c>
       <c r="G173" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H173" s="7"/>
       <c r="I173" s="2"/>
@@ -16060,16 +16048,16 @@
         <v>8</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F174" s="4">
         <v>1771</v>
       </c>
       <c r="G174" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H174" s="7"/>
       <c r="I174" s="2"/>
@@ -16127,16 +16115,16 @@
         <v>8</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F175" s="4">
         <v>1771</v>
       </c>
       <c r="G175" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H175" s="7"/>
       <c r="I175" s="2"/>
@@ -16196,16 +16184,16 @@
         <v>8</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F176" s="4">
         <v>1771</v>
       </c>
       <c r="G176" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H176" s="7"/>
       <c r="I176" s="2"/>
@@ -16265,16 +16253,16 @@
         <v>8</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F177" s="4">
         <v>1771</v>
       </c>
       <c r="G177" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H177" s="7"/>
       <c r="I177" s="2"/>
@@ -16332,16 +16320,16 @@
         <v>8</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E178" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F178" s="4">
         <v>1771</v>
       </c>
       <c r="G178" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H178" s="7"/>
       <c r="I178" s="2"/>
@@ -16401,16 +16389,16 @@
         <v>8</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F179" s="4">
         <v>1771</v>
       </c>
       <c r="G179" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H179" s="7"/>
       <c r="I179" s="2"/>
@@ -16470,16 +16458,16 @@
         <v>8</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F180" s="4">
         <v>1771</v>
       </c>
       <c r="G180" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H180" s="7"/>
       <c r="I180" s="2"/>
@@ -16539,16 +16527,16 @@
         <v>8</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F181" s="4">
         <v>1771</v>
       </c>
       <c r="G181" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H181" s="7"/>
       <c r="I181" s="2"/>
@@ -16608,16 +16596,16 @@
         <v>8</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F182" s="4">
         <v>1771</v>
       </c>
       <c r="G182" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H182" s="7"/>
       <c r="I182" s="2"/>
@@ -16677,16 +16665,16 @@
         <v>8</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F183" s="4">
         <v>1771</v>
       </c>
       <c r="G183" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H183" s="7"/>
       <c r="I183" s="2"/>
@@ -16744,16 +16732,16 @@
         <v>8</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F184" s="4">
         <v>1771</v>
       </c>
       <c r="G184" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H184" s="7"/>
       <c r="I184" s="2"/>
@@ -16811,16 +16799,16 @@
         <v>8</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F185" s="4">
         <v>1771</v>
       </c>
       <c r="G185" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H185" s="7"/>
       <c r="I185" s="2"/>
@@ -16880,16 +16868,16 @@
         <v>8</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E186" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F186" s="4">
         <v>1771</v>
       </c>
       <c r="G186" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H186" s="7"/>
       <c r="I186" s="2"/>
@@ -16947,16 +16935,16 @@
         <v>8</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E187" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F187" s="4">
         <v>1771</v>
       </c>
       <c r="G187" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H187" s="7"/>
       <c r="I187" s="2"/>
@@ -17014,16 +17002,16 @@
         <v>8</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E188" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F188" s="4">
         <v>1771</v>
       </c>
       <c r="G188" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H188" s="7"/>
       <c r="I188" s="2"/>
@@ -17081,16 +17069,16 @@
         <v>8</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E189" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F189" s="4">
         <v>1771</v>
       </c>
       <c r="G189" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H189" s="7"/>
       <c r="I189" s="2"/>
@@ -17148,16 +17136,16 @@
         <v>8</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E190" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F190" s="4">
         <v>1771</v>
       </c>
       <c r="G190" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H190" s="7"/>
       <c r="I190" s="2"/>
@@ -50186,10 +50174,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W2:W1148">
-    <cfRule type="cellIs" dxfId="6" priority="20" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="20" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="21" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="21" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>